<commit_message>
Add balance-sheet output Excel files
</commit_message>
<xml_diff>
--- a/output_Balance_Sheet_DS/CALIFORNIA_STATE_UNIVERSITY.xlsx
+++ b/output_Balance_Sheet_DS/CALIFORNIA_STATE_UNIVERSITY.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8330976</v>
+        <v>5793096</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2537878</v>
+        <v>2537879</v>
       </c>
     </row>
     <row r="7">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9300237000</v>
+        <v>9801435</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13964336</v>
+        <v>22820815</v>
       </c>
     </row>
     <row r="11">
@@ -581,9 +581,7 @@
           <t>net_assets_with_donor_restrictions</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>1488892</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -601,9 +599,7 @@
           <t>total_liabilities_and_net_assets</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>22262116</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>